<commit_message>
WIP Work in progress.
</commit_message>
<xml_diff>
--- a/Project/Datasets/Contenent Country List.xlsx
+++ b/Project/Datasets/Contenent Country List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonni\Desktop\EDA\Project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C52B297-0D83-4D4C-94FF-87933FB52608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F79D74E-E249-4FE1-A8F1-1A7384A1DF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7770" yWindow="-17985" windowWidth="19545" windowHeight="17040" xr2:uid="{529165A5-F640-4486-9B3C-675D4E4FE1A9}"/>
+    <workbookView xWindow="9225" yWindow="-21570" windowWidth="19485" windowHeight="17010" xr2:uid="{529165A5-F640-4486-9B3C-675D4E4FE1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="202">
   <si>
     <t>Country</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>United States of America</t>
+  </si>
+  <si>
+    <t>World</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EE4BBB-4546-44BE-B289-F7605A4F8E85}">
-  <dimension ref="A1:B194"/>
+  <dimension ref="A1:B195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2587,6 +2590,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>